<commit_message>
add column to provide link to NIST docs
</commit_message>
<xml_diff>
--- a/NNC-AWS-Config-TEMPLATE.xlsx
+++ b/NNC-AWS-Config-TEMPLATE.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkufro/Desktop/NNC/code/nnc-aws-rdk-controls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772B66E4-B1FE-6340-8638-CDD821510B87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC624D04-9621-BB43-942D-E18996264ECB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="480" windowWidth="31660" windowHeight="20540" xr2:uid="{5D2E16F2-8EC5-4504-9019-74D3240BE4C4}"/>
+    <workbookView xWindow="1940" yWindow="460" windowWidth="31660" windowHeight="20540" xr2:uid="{5D2E16F2-8EC5-4504-9019-74D3240BE4C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Control Family</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Test Type</t>
+  </si>
+  <si>
+    <t>Control Link</t>
   </si>
 </sst>
 </file>
@@ -440,11 +443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132045EB-EA2E-4606-A37F-0F4FB83EEC4E}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD56"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -452,18 +455,19 @@
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="61.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="52.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" customWidth="1"/>
-    <col min="11" max="11" width="23.83203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="66.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="72.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="61.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="66.1640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.83203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -477,32 +481,35 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{8B424400-2295-4A9D-937D-D38F028D7B00}"/>
+  <autoFilter ref="A1:M1" xr:uid="{8B424400-2295-4A9D-937D-D38F028D7B00}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>